<commit_message>
fix primaries, add spawn on clic for all species
</commit_message>
<xml_diff>
--- a/datafiles/genus.xlsx
+++ b/datafiles/genus.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d641367ab90122e/_tec/codi/GM/Terraformer2D/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="181" documentId="8_{9828CACF-C433-4BD3-8EC2-D880FF0C148B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{4BFF32D7-7175-46F0-A9F2-301CDE1DC688}"/>
+  <xr:revisionPtr revIDLastSave="191" documentId="8_{9828CACF-C433-4BD3-8EC2-D880FF0C148B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{FBFD9C5F-6685-4B5E-BD7F-DF962CA7BEAA}"/>
   <bookViews>
-    <workbookView xWindow="8355" yWindow="840" windowWidth="21225" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8145" yWindow="840" windowWidth="21225" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="initial_species" sheetId="3" r:id="rId1"/>
@@ -556,7 +556,207 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="10">
+  <dxfs count="30">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -961,7 +1161,7 @@
       <pane xSplit="1" ySplit="5" topLeftCell="B6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="N23" sqref="N23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1806,8 +2006,8 @@
       <c r="I25">
         <v>0</v>
       </c>
-      <c r="J25">
-        <v>0.1</v>
+      <c r="J25" s="8">
+        <v>0.3</v>
       </c>
       <c r="K25">
         <v>0.1</v>
@@ -1844,8 +2044,8 @@
       <c r="I26" s="1">
         <v>0.4</v>
       </c>
-      <c r="J26" s="1">
-        <v>0.12</v>
+      <c r="J26" s="9">
+        <v>0.05</v>
       </c>
       <c r="K26" s="1">
         <v>0.12</v>
@@ -2423,34 +2623,34 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K5">
-    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="19"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="L5">
-    <cfRule type="duplicateValues" dxfId="8" priority="8"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="F5">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="I5:L5 E5:G5 B5:C5">
-    <cfRule type="duplicateValues" dxfId="6" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G5 I5:J5 B5:C5 E5">
-    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="24"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="duplicateValues" dxfId="4" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="H5">
-    <cfRule type="duplicateValues" dxfId="3" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="15"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="duplicateValues" dxfId="2" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="D5">
-    <cfRule type="duplicateValues" dxfId="1" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C5">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="11"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
adjust carrying capacity for plants
</commit_message>
<xml_diff>
--- a/datafiles/genus.xlsx
+++ b/datafiles/genus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d641367ab90122e/_tec/codi/GM/Terraformer2D/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="8_{7DA26B0D-C8AE-4001-A03E-85F85492B8E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{B30AC750-6ED6-4187-8845-563F6B44835C}"/>
+  <xr:revisionPtr revIDLastSave="50" documentId="8_{7DA26B0D-C8AE-4001-A03E-85F85492B8E2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{6D872C3C-D5DE-4600-A0EC-B22FDF00854B}"/>
   <bookViews>
     <workbookView xWindow="5340" yWindow="300" windowWidth="21540" windowHeight="19170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -481,7 +481,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -549,7 +548,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -579,9 +578,6 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -592,6 +588,11 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1018,10 +1019,10 @@
   <dimension ref="A1:M51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="F20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="H35" sqref="H35"/>
+      <selection pane="bottomRight" activeCell="L30" sqref="L30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1034,9 +1035,9 @@
       <c r="A1" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="23">
+      <c r="B1" s="22">
         <f ca="1">NOW()</f>
-        <v>44323.655760300928</v>
+        <v>44325.979725810183</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -1057,14 +1058,14 @@
       <c r="B3" s="1">
         <v>0.1</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="21" t="s">
         <v>90</v>
       </c>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
+      <c r="J3" s="21"/>
+      <c r="K3" s="21"/>
+      <c r="L3" s="21"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1129,7 +1130,7 @@
       <c r="G6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="27" t="s">
         <v>83</v>
       </c>
       <c r="I6" s="11" t="s">
@@ -1158,7 +1159,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="4"/>
+      <c r="H7" s="25"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -1193,7 +1194,7 @@
         <f>VLOOKUP(G5,Tabla3[#All],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="2">
+      <c r="H8" s="26">
         <f>VLOOKUP(H5,Tabla3[#All],2,FALSE)</f>
         <v>0</v>
       </c>
@@ -1246,7 +1247,7 @@
         <f>VLOOKUP(G6,Tabla1[#All],2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="26">
         <f>VLOOKUP(H6,Tabla1[#All],2,FALSE)</f>
         <v>12</v>
       </c>
@@ -1539,7 +1540,7 @@
       <c r="G16">
         <v>0</v>
       </c>
-      <c r="H16" s="7">
+      <c r="H16" s="9">
         <v>1</v>
       </c>
       <c r="I16">
@@ -1675,7 +1676,7 @@
         <v>1</v>
       </c>
       <c r="L19">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="M19">
         <v>1</v>
@@ -1716,7 +1717,7 @@
         <v>2</v>
       </c>
       <c r="L20">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="M20">
         <v>1</v>
@@ -2003,7 +2004,7 @@
         <v>0.4</v>
       </c>
       <c r="L27">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="M27">
         <v>0.4</v>
@@ -2085,7 +2086,7 @@
         <v>0.05</v>
       </c>
       <c r="L29" s="1">
-        <v>0.12</v>
+        <v>0.05</v>
       </c>
       <c r="M29" s="1">
         <v>0.12</v>
@@ -2126,7 +2127,7 @@
         <v>0</v>
       </c>
       <c r="L30" s="8">
-        <v>0</v>
+        <v>15</v>
       </c>
       <c r="M30" s="8">
         <v>0</v>
@@ -2167,7 +2168,7 @@
         <v>50</v>
       </c>
       <c r="L31" s="8">
-        <v>50</v>
+        <v>15</v>
       </c>
       <c r="M31" s="8">
         <v>50</v>
@@ -2195,7 +2196,7 @@
       <c r="G32" s="1">
         <v>0</v>
       </c>
-      <c r="H32" s="8">
+      <c r="H32" s="10">
         <v>0</v>
       </c>
       <c r="I32" s="1">
@@ -2236,7 +2237,7 @@
       <c r="G33" s="10">
         <v>0.9</v>
       </c>
-      <c r="H33" s="8">
+      <c r="H33" s="10">
         <v>0.7</v>
       </c>
       <c r="I33" s="10">
@@ -2277,7 +2278,7 @@
       <c r="G34" s="1">
         <v>0</v>
       </c>
-      <c r="H34" s="8">
+      <c r="H34" s="10">
         <v>0</v>
       </c>
       <c r="I34" s="1">
@@ -2522,7 +2523,7 @@
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
       <c r="G43" s="4"/>
-      <c r="H43" s="18"/>
+      <c r="H43" s="17"/>
       <c r="I43" s="4"/>
       <c r="J43" s="4"/>
       <c r="K43" s="4"/>
@@ -2539,7 +2540,7 @@
       <c r="F44" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="H44" s="19"/>
+      <c r="H44" s="18"/>
       <c r="J44" s="6" t="s">
         <v>50</v>
       </c>
@@ -2554,39 +2555,39 @@
       <c r="A47" t="s">
         <v>42</v>
       </c>
-      <c r="B47" s="21">
+      <c r="B47" s="20">
         <f>+B29/B35/B15/$B$3</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C47" s="21">
+      <c r="C47" s="20">
         <f t="shared" ref="C47:J47" si="0">+C29/C35/C15/$B$3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D47" s="21">
+      <c r="D47" s="20">
         <f t="shared" si="0"/>
         <v>0.59999999999999987</v>
       </c>
-      <c r="E47" s="21">
+      <c r="E47" s="20">
         <f t="shared" si="0"/>
         <v>4.4444444444444446</v>
       </c>
-      <c r="F47" s="21">
+      <c r="F47" s="20">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G47" s="21">
+      <c r="G47" s="20">
         <f t="shared" si="0"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="H47" s="21">
+      <c r="H47" s="20">
         <f t="shared" si="0"/>
         <v>8.5470085470085472E-2</v>
       </c>
-      <c r="I47" s="21">
+      <c r="I47" s="20">
         <f t="shared" si="0"/>
         <v>3.333333333333333</v>
       </c>
-      <c r="J47" s="20">
+      <c r="J47" s="19">
         <f t="shared" si="0"/>
         <v>3.333333333333333</v>
       </c>
@@ -2598,39 +2599,39 @@
       <c r="A49" t="s">
         <v>87</v>
       </c>
-      <c r="B49" s="24">
+      <c r="B49" s="23">
         <f t="shared" ref="B49:G49" si="1">+B47*B24*$B$3*$B$2</f>
         <v>2400</v>
       </c>
-      <c r="C49" s="24">
+      <c r="C49" s="23">
         <f t="shared" si="1"/>
         <v>1500</v>
       </c>
-      <c r="D49" s="24">
+      <c r="D49" s="23">
         <f t="shared" si="1"/>
         <v>2159.9999999999995</v>
       </c>
-      <c r="E49" s="24">
+      <c r="E49" s="23">
         <f t="shared" si="1"/>
         <v>24000</v>
       </c>
-      <c r="F49" s="24">
+      <c r="F49" s="23">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="G49" s="24">
+      <c r="G49" s="23">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="H49" s="24">
+      <c r="H49" s="23">
         <f>+H47*H24*$B$3*$B$2</f>
         <v>615.38461538461547</v>
       </c>
-      <c r="I49" s="24">
+      <c r="I49" s="23">
         <f t="shared" ref="I49:J49" si="2">+I47*I24*$B$3*$B$2</f>
         <v>600</v>
       </c>
-      <c r="J49" s="24">
+      <c r="J49" s="23">
         <f t="shared" si="2"/>
         <v>600</v>
       </c>
@@ -2639,39 +2640,39 @@
       <c r="A50" t="s">
         <v>89</v>
       </c>
-      <c r="B50" s="25">
+      <c r="B50" s="24">
         <f t="shared" ref="B50:G50" si="3">+B35*B47*$B$3*B15*B24</f>
         <v>160</v>
       </c>
-      <c r="C50" s="25">
+      <c r="C50" s="24">
         <f t="shared" si="3"/>
         <v>2.5</v>
       </c>
-      <c r="D50" s="25">
+      <c r="D50" s="24">
         <f t="shared" si="3"/>
         <v>17.999999999999996</v>
       </c>
-      <c r="E50" s="25">
+      <c r="E50" s="24">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
-      <c r="F50" s="25">
+      <c r="F50" s="24">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="G50" s="25">
+      <c r="G50" s="24">
         <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
-      <c r="H50" s="25">
+      <c r="H50" s="24">
         <f>+H35*H47*$B$3*H15*H24</f>
         <v>80</v>
       </c>
-      <c r="I50" s="25">
+      <c r="I50" s="24">
         <f t="shared" ref="I50:J50" si="4">+I35*I47*$B$3*I15*I24</f>
         <v>4</v>
       </c>
-      <c r="J50" s="25">
+      <c r="J50" s="24">
         <f t="shared" si="4"/>
         <v>4</v>
       </c>
@@ -2680,39 +2681,39 @@
       <c r="A51" t="s">
         <v>86</v>
       </c>
-      <c r="B51" s="25">
+      <c r="B51" s="24">
         <f t="shared" ref="B51:G51" si="5">+B29*B24</f>
         <v>160</v>
       </c>
-      <c r="C51" s="25">
+      <c r="C51" s="24">
         <f t="shared" si="5"/>
         <v>2.5</v>
       </c>
-      <c r="D51" s="25">
+      <c r="D51" s="24">
         <f t="shared" si="5"/>
         <v>18</v>
       </c>
-      <c r="E51" s="25">
+      <c r="E51" s="24">
         <f t="shared" si="5"/>
         <v>240</v>
       </c>
-      <c r="F51" s="25">
+      <c r="F51" s="24">
         <f t="shared" si="5"/>
         <v>0.8</v>
       </c>
-      <c r="G51" s="25">
+      <c r="G51" s="24">
         <f t="shared" si="5"/>
         <v>1.6</v>
       </c>
-      <c r="H51" s="25">
+      <c r="H51" s="24">
         <f>+H29*H24</f>
         <v>80</v>
       </c>
-      <c r="I51" s="25">
+      <c r="I51" s="24">
         <f t="shared" ref="I51:J51" si="6">+I29*I24</f>
         <v>4</v>
       </c>
-      <c r="J51" s="25">
+      <c r="J51" s="24">
         <f t="shared" si="6"/>
         <v>4</v>
       </c>
@@ -2759,7 +2760,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" disablePrompts="1" count="2">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{B3D47E63-4CCF-498A-86C2-6290C49D352E}">
           <x14:formula1>
             <xm:f>Tables!$A$4:$A$21</xm:f>

</xml_diff>

<commit_message>
unified structure_metabolism for plants and animals
</commit_message>
<xml_diff>
--- a/datafiles/genus.xlsx
+++ b/datafiles/genus.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/8d641367ab90122e/_tec/codi/GM/Terraformer2D/datafiles/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="23" documentId="8_{28B0AFDC-BCC3-475A-8C86-8E0ED1EF7BA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{D1065056-ABDD-47AB-A527-A11BF24291A4}"/>
+  <xr:revisionPtr revIDLastSave="45" documentId="8_{28B0AFDC-BCC3-475A-8C86-8E0ED1EF7BA8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{31EE5506-B7C2-48E3-9D00-A4B092FAF7FA}"/>
   <bookViews>
     <workbookView xWindow="5340" yWindow="300" windowWidth="21540" windowHeight="19170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -118,7 +118,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="96">
   <si>
     <t>GEN_START</t>
   </si>
@@ -207,9 +207,6 @@
     <t>SPECIE_CODE</t>
   </si>
   <si>
-    <t>ANIMAL_ANABOLISM_BIOMASS_CONVERSION</t>
-  </si>
-  <si>
     <t>BIOMASS_BIRTH</t>
   </si>
   <si>
@@ -403,6 +400,12 @@
   </si>
   <si>
     <t>Primary tiny 2</t>
+  </si>
+  <si>
+    <t>KA_ANABOLISM_FACTOR</t>
+  </si>
+  <si>
+    <t>EMPTY14</t>
   </si>
 </sst>
 </file>
@@ -557,7 +560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -588,7 +591,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1051,10 +1053,10 @@
   <dimension ref="A1:N51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="6" topLeftCell="F7" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="6" topLeftCell="B19" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
-      <selection pane="bottomRight" activeCell="M29" sqref="M29"/>
+      <selection pane="bottomRight" activeCell="H29" sqref="H29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1066,44 +1068,44 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>92</v>
-      </c>
-      <c r="B1" s="21">
+        <v>91</v>
+      </c>
+      <c r="B1" s="20">
         <f ca="1">NOW()</f>
-        <v>44327.047491087964</v>
+        <v>44328.150702662038</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B2" s="8">
         <v>180</v>
       </c>
       <c r="G2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B3" s="1">
         <v>0.1</v>
       </c>
-      <c r="G3" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="H3" s="20"/>
-      <c r="I3" s="20"/>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="20"/>
+      <c r="G3" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="H3" s="19"/>
+      <c r="I3" s="19"/>
+      <c r="J3" s="19"/>
+      <c r="K3" s="19"/>
+      <c r="L3" s="19"/>
+      <c r="M3" s="19"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B5" s="5" t="s">
         <v>8</v>
@@ -1147,34 +1149,34 @@
     </row>
     <row r="6" spans="1:14" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E6" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>41</v>
+        <v>58</v>
+      </c>
+      <c r="F6" s="26" t="s">
+        <v>40</v>
       </c>
       <c r="G6" s="12" t="s">
         <v>12</v>
       </c>
-      <c r="H6" s="26" t="s">
-        <v>82</v>
+      <c r="H6" s="25" t="s">
+        <v>81</v>
       </c>
       <c r="I6" s="11" t="s">
         <v>13</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="K6" s="11" t="s">
         <v>15</v>
@@ -1183,7 +1185,7 @@
         <v>14</v>
       </c>
       <c r="M6" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="N6" s="11" t="s">
         <v>3</v>
@@ -1199,7 +1201,7 @@
       <c r="E7" s="4"/>
       <c r="F7" s="4"/>
       <c r="G7" s="4"/>
-      <c r="H7" s="24"/>
+      <c r="H7" s="23"/>
       <c r="I7" s="4"/>
       <c r="J7" s="4"/>
       <c r="K7" s="4"/>
@@ -1235,7 +1237,7 @@
         <f>VLOOKUP(G5,Tabla3[#All],2,FALSE)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="25">
+      <c r="H8" s="24">
         <f>VLOOKUP(H5,Tabla3[#All],2,FALSE)</f>
         <v>0</v>
       </c>
@@ -1266,7 +1268,7 @@
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B9" s="2">
         <f>VLOOKUP(B6,Tabla1[#All],2,FALSE)</f>
@@ -1292,7 +1294,7 @@
         <f>VLOOKUP(G6,Tabla1[#All],2,FALSE)</f>
         <v>4</v>
       </c>
-      <c r="H9" s="25">
+      <c r="H9" s="24">
         <f>VLOOKUP(H6,Tabla1[#All],2,FALSE)</f>
         <v>12</v>
       </c>
@@ -1323,34 +1325,34 @@
     </row>
     <row r="10" spans="1:14" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>16</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G10" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="H10" s="28" t="s">
-        <v>83</v>
+      <c r="H10" s="27" t="s">
+        <v>82</v>
       </c>
       <c r="I10" s="6" t="s">
         <v>18</v>
       </c>
       <c r="J10" s="6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="K10" s="6" t="s">
         <v>19</v>
@@ -1359,7 +1361,7 @@
         <v>20</v>
       </c>
       <c r="M10" s="6" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="N10" s="6" t="s">
         <v>21</v>
@@ -1455,7 +1457,7 @@
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B13">
         <v>-1</v>
@@ -1543,7 +1545,7 @@
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B15">
         <v>30</v>
@@ -1587,7 +1589,7 @@
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B16">
         <v>0</v>
@@ -1763,7 +1765,7 @@
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B20">
         <v>1</v>
@@ -1807,7 +1809,7 @@
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -1851,7 +1853,7 @@
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B22">
         <v>3</v>
@@ -1895,7 +1897,7 @@
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B23">
         <v>3</v>
@@ -1939,7 +1941,7 @@
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B24">
         <v>800</v>
@@ -1983,7 +1985,7 @@
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -2071,7 +2073,7 @@
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B27">
         <v>0.4</v>
@@ -2115,34 +2117,34 @@
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>29</v>
-      </c>
-      <c r="B28">
-        <v>0</v>
-      </c>
-      <c r="C28">
-        <v>0</v>
-      </c>
-      <c r="D28">
-        <v>0</v>
-      </c>
-      <c r="E28">
-        <v>0</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-      <c r="G28">
-        <v>0</v>
-      </c>
-      <c r="H28" s="9">
-        <v>0</v>
-      </c>
-      <c r="I28">
-        <v>0</v>
-      </c>
-      <c r="J28">
-        <v>0</v>
+        <v>94</v>
+      </c>
+      <c r="B28" s="1">
+        <v>0.4</v>
+      </c>
+      <c r="C28" s="1">
+        <v>0.01</v>
+      </c>
+      <c r="D28" s="1">
+        <v>0.05</v>
+      </c>
+      <c r="E28" s="1">
+        <v>0.06</v>
+      </c>
+      <c r="F28" s="1">
+        <v>1</v>
+      </c>
+      <c r="G28" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="H28" s="10">
+        <v>0.17</v>
+      </c>
+      <c r="I28" s="1">
+        <v>0.04</v>
+      </c>
+      <c r="J28" s="1">
+        <v>0.04</v>
       </c>
       <c r="K28" s="7">
         <v>0.3</v>
@@ -2159,7 +2161,7 @@
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B29" s="1">
         <v>0.2</v>
@@ -2203,7 +2205,7 @@
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B30" s="1">
         <v>30</v>
@@ -2247,7 +2249,7 @@
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B31" s="1">
         <v>15</v>
@@ -2291,7 +2293,7 @@
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -2335,7 +2337,7 @@
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="9" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B33" s="10">
         <v>0.9</v>
@@ -2379,7 +2381,7 @@
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -2422,52 +2424,52 @@
       </c>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>33</v>
-      </c>
-      <c r="B35" s="1">
-        <v>0.4</v>
-      </c>
-      <c r="C35" s="1">
-        <v>0.01</v>
-      </c>
-      <c r="D35" s="1">
-        <v>0.05</v>
-      </c>
-      <c r="E35" s="1">
-        <v>0.06</v>
-      </c>
-      <c r="F35" s="1">
-        <v>1</v>
-      </c>
-      <c r="G35" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="H35" s="10">
-        <v>0.13</v>
-      </c>
-      <c r="I35" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="J35" s="1">
-        <v>0.04</v>
-      </c>
-      <c r="K35">
-        <v>0</v>
-      </c>
-      <c r="L35">
-        <v>0</v>
-      </c>
-      <c r="M35">
-        <v>0</v>
-      </c>
-      <c r="N35">
+      <c r="A35" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="B35" s="7">
+        <v>0</v>
+      </c>
+      <c r="C35" s="7">
+        <v>0</v>
+      </c>
+      <c r="D35" s="7">
+        <v>0</v>
+      </c>
+      <c r="E35" s="7">
+        <v>0</v>
+      </c>
+      <c r="F35" s="7">
+        <v>0</v>
+      </c>
+      <c r="G35" s="7">
+        <v>0</v>
+      </c>
+      <c r="H35" s="7">
+        <v>0</v>
+      </c>
+      <c r="I35" s="7">
+        <v>0</v>
+      </c>
+      <c r="J35" s="7">
+        <v>0</v>
+      </c>
+      <c r="K35" s="7">
+        <v>0</v>
+      </c>
+      <c r="L35" s="7">
+        <v>0</v>
+      </c>
+      <c r="M35" s="7">
+        <v>0</v>
+      </c>
+      <c r="N35" s="7">
         <v>0</v>
       </c>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B36" s="1">
         <v>1600</v>
@@ -2511,7 +2513,7 @@
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B37" s="1">
         <v>1.2</v>
@@ -2555,7 +2557,7 @@
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B38" s="1">
         <v>50</v>
@@ -2599,7 +2601,7 @@
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B39" s="1">
         <v>1</v>
@@ -2672,17 +2674,17 @@
     </row>
     <row r="44" spans="1:14" s="6" customFormat="1" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="E44" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="F44" s="6" t="s">
         <v>48</v>
-      </c>
-      <c r="E44" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>49</v>
       </c>
       <c r="H44" s="17"/>
       <c r="J44" s="6" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
@@ -2693,37 +2695,37 @@
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>42</v>
-      </c>
-      <c r="B47" s="19">
-        <f>+B29/B35/B15/$B$3</f>
+        <v>41</v>
+      </c>
+      <c r="B47" s="18">
+        <f>+B29/B28/B15/$B$3</f>
         <v>0.16666666666666666</v>
       </c>
-      <c r="C47" s="19">
-        <f t="shared" ref="C47:J47" si="0">+C29/C35/C15/$B$3</f>
+      <c r="C47" s="18">
+        <f t="shared" ref="C47:N47" si="0">+C29/C28/C15/$B$3</f>
         <v>0.33333333333333331</v>
       </c>
-      <c r="D47" s="19">
+      <c r="D47" s="18">
         <f t="shared" si="0"/>
         <v>0.59999999999999987</v>
       </c>
-      <c r="E47" s="19">
+      <c r="E47" s="18">
         <f t="shared" si="0"/>
         <v>4.4444444444444446</v>
       </c>
-      <c r="F47" s="19">
+      <c r="F47" s="18">
         <f t="shared" si="0"/>
         <v>0.33333333333333331</v>
       </c>
-      <c r="G47" s="19">
+      <c r="G47" s="18">
         <f t="shared" si="0"/>
         <v>1.6666666666666665</v>
       </c>
-      <c r="H47" s="19">
+      <c r="H47" s="18">
         <f t="shared" si="0"/>
-        <v>8.5470085470085472E-2</v>
-      </c>
-      <c r="I47" s="19">
+        <v>6.535947712418301E-2</v>
+      </c>
+      <c r="I47" s="18">
         <f t="shared" si="0"/>
         <v>3.333333333333333</v>
       </c>
@@ -2731,130 +2733,146 @@
         <f t="shared" si="0"/>
         <v>3.333333333333333</v>
       </c>
+      <c r="K47" s="18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="L47" s="18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="M47" s="18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
+      <c r="N47" s="18" t="e">
+        <f t="shared" si="0"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="H48" s="7"/>
     </row>
     <row r="49" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>86</v>
-      </c>
-      <c r="B49" s="22">
+        <v>85</v>
+      </c>
+      <c r="B49" s="21">
         <f t="shared" ref="B49:G49" si="1">+B47*B24*$B$3*$B$2</f>
         <v>2400</v>
       </c>
-      <c r="C49" s="22">
+      <c r="C49" s="21">
         <f t="shared" si="1"/>
         <v>1500</v>
       </c>
-      <c r="D49" s="22">
+      <c r="D49" s="21">
         <f t="shared" si="1"/>
         <v>2159.9999999999995</v>
       </c>
-      <c r="E49" s="22">
+      <c r="E49" s="21">
         <f t="shared" si="1"/>
         <v>24000</v>
       </c>
-      <c r="F49" s="22">
+      <c r="F49" s="21">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="G49" s="22">
+      <c r="G49" s="21">
         <f t="shared" si="1"/>
         <v>240</v>
       </c>
-      <c r="H49" s="22">
+      <c r="H49" s="21">
         <f>+H47*H24*$B$3*$B$2</f>
-        <v>615.38461538461547</v>
-      </c>
-      <c r="I49" s="22">
+        <v>470.58823529411774</v>
+      </c>
+      <c r="I49" s="21">
         <f t="shared" ref="I49:J49" si="2">+I47*I24*$B$3*$B$2</f>
         <v>600</v>
       </c>
-      <c r="J49" s="22">
+      <c r="J49" s="21">
         <f t="shared" si="2"/>
         <v>600</v>
       </c>
     </row>
     <row r="50" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>88</v>
-      </c>
-      <c r="B50" s="23">
-        <f t="shared" ref="B50:G50" si="3">+B35*B47*$B$3*B15*B24</f>
+        <v>87</v>
+      </c>
+      <c r="B50" s="22">
+        <f>+B28*B47*$B$3*B15*B24</f>
         <v>160</v>
       </c>
-      <c r="C50" s="23">
-        <f t="shared" si="3"/>
+      <c r="C50" s="22">
+        <f t="shared" ref="C50:J50" si="3">+C28*C47*$B$3*C15*C24</f>
         <v>2.5</v>
       </c>
-      <c r="D50" s="23">
+      <c r="D50" s="22">
         <f t="shared" si="3"/>
         <v>17.999999999999996</v>
       </c>
-      <c r="E50" s="23">
+      <c r="E50" s="22">
         <f t="shared" si="3"/>
         <v>240</v>
       </c>
-      <c r="F50" s="23">
+      <c r="F50" s="22">
         <f t="shared" si="3"/>
         <v>0.8</v>
       </c>
-      <c r="G50" s="23">
+      <c r="G50" s="22">
         <f t="shared" si="3"/>
         <v>1.6</v>
       </c>
-      <c r="H50" s="23">
-        <f>+H35*H47*$B$3*H15*H24</f>
-        <v>80</v>
-      </c>
-      <c r="I50" s="23">
-        <f t="shared" ref="I50:J50" si="4">+I35*I47*$B$3*I15*I24</f>
+      <c r="H50" s="22">
+        <f t="shared" si="3"/>
+        <v>80.000000000000014</v>
+      </c>
+      <c r="I50" s="22">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="J50" s="23">
-        <f t="shared" si="4"/>
+      <c r="J50" s="22">
+        <f t="shared" si="3"/>
         <v>4</v>
       </c>
     </row>
     <row r="51" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>85</v>
-      </c>
-      <c r="B51" s="23">
-        <f t="shared" ref="B51:G51" si="5">+B29*B24</f>
+        <v>84</v>
+      </c>
+      <c r="B51" s="22">
+        <f t="shared" ref="B51:G51" si="4">+B29*B24</f>
         <v>160</v>
       </c>
-      <c r="C51" s="23">
-        <f t="shared" si="5"/>
+      <c r="C51" s="22">
+        <f t="shared" si="4"/>
         <v>2.5</v>
       </c>
-      <c r="D51" s="23">
-        <f t="shared" si="5"/>
+      <c r="D51" s="22">
+        <f t="shared" si="4"/>
         <v>18</v>
       </c>
-      <c r="E51" s="23">
-        <f t="shared" si="5"/>
+      <c r="E51" s="22">
+        <f t="shared" si="4"/>
         <v>240</v>
       </c>
-      <c r="F51" s="23">
-        <f t="shared" si="5"/>
+      <c r="F51" s="22">
+        <f t="shared" si="4"/>
         <v>0.8</v>
       </c>
-      <c r="G51" s="23">
-        <f t="shared" si="5"/>
+      <c r="G51" s="22">
+        <f t="shared" si="4"/>
         <v>1.6</v>
       </c>
-      <c r="H51" s="23">
+      <c r="H51" s="22">
         <f>+H29*H24</f>
         <v>80</v>
       </c>
-      <c r="I51" s="23">
-        <f t="shared" ref="I51:J51" si="6">+I29*I24</f>
+      <c r="I51" s="22">
+        <f t="shared" ref="I51:J51" si="5">+I29*I24</f>
         <v>4</v>
       </c>
-      <c r="J51" s="23">
-        <f t="shared" si="6"/>
+      <c r="J51" s="22">
+        <f t="shared" si="5"/>
         <v>4</v>
       </c>
     </row>
@@ -2968,7 +2986,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -2976,7 +2994,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8">
         <v>3</v>
@@ -3024,7 +3042,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B14">
         <v>9</v>
@@ -3032,7 +3050,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B15">
         <v>10</v>
@@ -3040,7 +3058,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B16">
         <v>11</v>
@@ -3048,7 +3066,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17">
         <v>12</v>
@@ -3056,7 +3074,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B18">
         <v>13</v>
@@ -3064,7 +3082,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B19">
         <v>14</v>
@@ -3072,7 +3090,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B20">
         <v>15</v>
@@ -3080,7 +3098,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B21">
         <v>99</v>
@@ -3139,21 +3157,21 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
+        <v>74</v>
+      </c>
+      <c r="C1" t="s">
         <v>75</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1" t="s">
+        <v>74</v>
+      </c>
+      <c r="F1" t="s">
         <v>76</v>
-      </c>
-      <c r="E1" t="s">
-        <v>75</v>
-      </c>
-      <c r="F1" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B2">
         <v>0</v>
@@ -3170,7 +3188,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B3">
         <v>1.5</v>
@@ -3187,7 +3205,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B4">
         <v>2.5</v>
@@ -3204,7 +3222,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B5">
         <v>9999999</v>
@@ -3221,19 +3239,19 @@
     </row>
     <row r="10" spans="1:7" s="6" customFormat="1" ht="60" x14ac:dyDescent="0.25">
       <c r="B10" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E10" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F10" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G10" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="G10" s="6" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>